<commit_message>
Modify top10 for less than 10
</commit_message>
<xml_diff>
--- a/fund/data.xlsx
+++ b/fund/data.xlsx
@@ -619,7 +619,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
@@ -632,6 +632,18 @@
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="center" wrapText="1"/>
@@ -1152,37 +1164,37 @@
       </c>
     </row>
     <row r="2" ht="175" customHeight="1">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>富国内需增长混合</t>
         </is>
       </c>
-      <c r="B2" s="6" t="inlineStr">
+      <c r="B2" s="10" t="inlineStr">
         <is>
           <t>008901</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="9" t="inlineStr">
         <is>
           <t>1.9731</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="D2" s="9" t="inlineStr">
         <is>
           <t>+2.99%</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="E2" s="9" t="inlineStr">
         <is>
           <t>1.9706</t>
         </is>
       </c>
-      <c r="F2" s="7" t="inlineStr">
+      <c r="F2" s="11" t="inlineStr">
         <is>
           <t>2.86%</t>
         </is>
       </c>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="9" t="inlineStr">
         <is>
           <t>贵州茅台 8.81% 5.89% 
 伊利股份 8.80% 1.02% 
@@ -1198,7 +1210,7 @@
 持仓截止日期: 2020-12-31</t>
         </is>
       </c>
-      <c r="H2" s="5" t="inlineStr">
+      <c r="H2" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">02-10 1.9706 2.86% 
 02-09 1.9158 1.70% 
@@ -1213,27 +1225,27 @@
 </t>
         </is>
       </c>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="I2" s="9" t="inlineStr">
         <is>
           <t>王园园</t>
         </is>
       </c>
-      <c r="J2" s="8" t="inlineStr">
+      <c r="J2" s="12" t="inlineStr">
         <is>
           <t>2020-03-26</t>
         </is>
       </c>
-      <c r="K2" s="8" t="inlineStr">
+      <c r="K2" s="12" t="inlineStr">
         <is>
           <t>2020-12-31</t>
         </is>
       </c>
-      <c r="L2" s="5" t="inlineStr">
+      <c r="L2" s="9" t="inlineStr">
         <is>
           <t>23.02亿元</t>
         </is>
       </c>
-      <c r="M2" s="5" t="inlineStr">
+      <c r="M2" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">2020-12-31 23.02 
 2020-09-30 30.84 
@@ -1242,46 +1254,46 @@
 </t>
         </is>
       </c>
-      <c r="N2" s="5" t="inlineStr">
+      <c r="N2" s="9" t="inlineStr">
         <is>
           <t>2020-06-30: 145.10%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="inlineStr">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>国寿安保泰吉纯债一年定开债</t>
         </is>
       </c>
-      <c r="B3" s="6" t="inlineStr">
+      <c r="B3" s="10" t="inlineStr">
         <is>
           <t>008902</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr">
+      <c r="C3" s="9" t="inlineStr">
         <is>
           <t>--</t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr"/>
-      <c r="E3" s="5" t="inlineStr">
+      <c r="D3" s="9" t="inlineStr"/>
+      <c r="E3" s="9" t="inlineStr">
         <is>
           <t>0.9991</t>
         </is>
       </c>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="F3" s="9" t="inlineStr">
         <is>
           <t>--</t>
         </is>
       </c>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">
 </t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
+      <c r="H3" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">02-10 0.9991 -- 
 02-05 0.9985 -- 
@@ -1296,27 +1308,27 @@
 </t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr">
+      <c r="I3" s="9" t="inlineStr">
         <is>
           <t>陶尹斌</t>
         </is>
       </c>
-      <c r="J3" s="5" t="inlineStr">
+      <c r="J3" s="9" t="inlineStr">
         <is>
           <t>2020-03-16</t>
         </is>
       </c>
-      <c r="K3" s="5" t="inlineStr">
+      <c r="K3" s="9" t="inlineStr">
         <is>
           <t>2020-12-31</t>
         </is>
       </c>
-      <c r="L3" s="5" t="inlineStr">
+      <c r="L3" s="9" t="inlineStr">
         <is>
           <t>9.97亿元</t>
         </is>
       </c>
-      <c r="M3" s="5" t="inlineStr">
+      <c r="M3" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">2020-12-31 9.97 
 2020-09-30 9.87 
@@ -1325,40 +1337,40 @@
 </t>
         </is>
       </c>
-      <c r="N3" s="5" t="inlineStr"/>
+      <c r="N3" s="9" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="inlineStr">
+      <c r="A4" s="9" t="inlineStr">
         <is>
           <t>广发科技先锋混合</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr">
+      <c r="B4" s="10" t="inlineStr">
         <is>
           <t>008903</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
+      <c r="C4" s="9" t="inlineStr">
         <is>
           <t>1.8532</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
+      <c r="D4" s="9" t="inlineStr">
         <is>
           <t>+4.02%</t>
         </is>
       </c>
-      <c r="E4" s="5" t="inlineStr">
+      <c r="E4" s="9" t="inlineStr">
         <is>
           <t>1.8437</t>
         </is>
       </c>
-      <c r="F4" s="5" t="inlineStr">
+      <c r="F4" s="9" t="inlineStr">
         <is>
           <t>3.49%</t>
         </is>
       </c>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G4" s="9" t="inlineStr">
         <is>
           <t>亿纬锂能 10.05% 5.21% 
 隆基股份 9.74% 3.89% 
@@ -1374,7 +1386,7 @@
 持仓截止日期: 2020-12-31</t>
         </is>
       </c>
-      <c r="H4" s="5" t="inlineStr">
+      <c r="H4" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">02-10 1.8437 3.49% 
 02-09 1.7815 3.38% 
@@ -1389,27 +1401,27 @@
 </t>
         </is>
       </c>
-      <c r="I4" s="5" t="inlineStr">
+      <c r="I4" s="9" t="inlineStr">
         <is>
           <t>刘格菘</t>
         </is>
       </c>
-      <c r="J4" s="5" t="inlineStr">
+      <c r="J4" s="9" t="inlineStr">
         <is>
           <t>2020-01-22</t>
         </is>
       </c>
-      <c r="K4" s="5" t="inlineStr">
+      <c r="K4" s="9" t="inlineStr">
         <is>
           <t>2020-12-31</t>
         </is>
       </c>
-      <c r="L4" s="5" t="inlineStr">
+      <c r="L4" s="9" t="inlineStr">
         <is>
           <t>239.70亿元</t>
         </is>
       </c>
-      <c r="M4" s="5" t="inlineStr">
+      <c r="M4" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">2020-12-31 239.70 
 2020-09-30 236.87 
@@ -1419,50 +1431,50 @@
 </t>
         </is>
       </c>
-      <c r="N4" s="5" t="inlineStr">
+      <c r="N4" s="9" t="inlineStr">
         <is>
           <t>2020-06-30: 193.64%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="inlineStr">
+      <c r="A5" s="9" t="inlineStr">
         <is>
           <t>华安安腾一年定开债</t>
         </is>
       </c>
-      <c r="B5" s="6" t="inlineStr">
+      <c r="B5" s="10" t="inlineStr">
         <is>
           <t>008904</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr">
+      <c r="C5" s="9" t="inlineStr">
         <is>
           <t>1.0006</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
+      <c r="D5" s="9" t="inlineStr">
         <is>
           <t>+0.05%</t>
         </is>
       </c>
-      <c r="E5" s="5" t="inlineStr">
+      <c r="E5" s="9" t="inlineStr">
         <is>
           <t>1.0004</t>
         </is>
       </c>
-      <c r="F5" s="5" t="inlineStr">
+      <c r="F5" s="9" t="inlineStr">
         <is>
           <t>0.03%</t>
         </is>
       </c>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="G5" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">
 </t>
         </is>
       </c>
-      <c r="H5" s="5" t="inlineStr">
+      <c r="H5" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">02-10 1.0004 0.03% 
 02-09 1.0001 0.02% 
@@ -1477,27 +1489,27 @@
 </t>
         </is>
       </c>
-      <c r="I5" s="5" t="inlineStr">
+      <c r="I5" s="9" t="inlineStr">
         <is>
           <t>马晓璇</t>
         </is>
       </c>
-      <c r="J5" s="5" t="inlineStr">
+      <c r="J5" s="9" t="inlineStr">
         <is>
           <t>2020-04-22</t>
         </is>
       </c>
-      <c r="K5" s="5" t="inlineStr">
+      <c r="K5" s="9" t="inlineStr">
         <is>
           <t>2020-12-31</t>
         </is>
       </c>
-      <c r="L5" s="5" t="inlineStr">
+      <c r="L5" s="9" t="inlineStr">
         <is>
           <t>5.09亿元</t>
         </is>
       </c>
-      <c r="M5" s="5" t="inlineStr">
+      <c r="M5" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">2020-12-31 5.09 
 2020-09-30 5.05 
@@ -1506,46 +1518,51 @@
 </t>
         </is>
       </c>
-      <c r="N5" s="5" t="inlineStr"/>
+      <c r="N5" s="9" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="inlineStr">
+      <c r="A6" s="9" t="inlineStr">
         <is>
           <t>嘉合锦鹏添利混合A</t>
         </is>
       </c>
-      <c r="B6" s="6" t="inlineStr">
+      <c r="B6" s="10" t="inlineStr">
         <is>
           <t>008905</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr">
+      <c r="C6" s="9" t="inlineStr">
         <is>
           <t>1.0078</t>
         </is>
       </c>
-      <c r="D6" s="5" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>+0.09%</t>
         </is>
       </c>
-      <c r="E6" s="5" t="inlineStr">
+      <c r="E6" s="9" t="inlineStr">
         <is>
           <t>1.0073</t>
         </is>
       </c>
-      <c r="F6" s="5" t="inlineStr">
+      <c r="F6" s="9" t="inlineStr">
         <is>
           <t>0.04%</t>
         </is>
       </c>
-      <c r="G6" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-</t>
-        </is>
-      </c>
-      <c r="H6" s="5" t="inlineStr">
+      <c r="G6" s="9" t="inlineStr">
+        <is>
+          <t>工商银行 1.08% 1.94% 
+中国建筑 1.08% 0.00% 
+浦发银行 1.05% 0.09% 
+中国化学 1.02% 0.64% 
+兖州煤业 0.87% 1.49% 
+前十持仓占比合计：5.10%
+持仓截止日期: 2020-12-31</t>
+        </is>
+      </c>
+      <c r="H6" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">02-10 1.0073 0.04% 
 02-09 1.0069 0.18% 
@@ -1560,27 +1577,27 @@
 </t>
         </is>
       </c>
-      <c r="I6" s="5" t="inlineStr">
+      <c r="I6" s="9" t="inlineStr">
         <is>
           <t>于启明</t>
         </is>
       </c>
-      <c r="J6" s="5" t="inlineStr">
+      <c r="J6" s="9" t="inlineStr">
         <is>
           <t>2020-04-29</t>
         </is>
       </c>
-      <c r="K6" s="5" t="inlineStr">
+      <c r="K6" s="9" t="inlineStr">
         <is>
           <t>2020-12-31</t>
         </is>
       </c>
-      <c r="L6" s="5" t="inlineStr">
+      <c r="L6" s="9" t="inlineStr">
         <is>
           <t>1.91亿元</t>
         </is>
       </c>
-      <c r="M6" s="5" t="inlineStr">
+      <c r="M6" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">2020-12-31 1.91 
 2020-09-30 3.04 
@@ -1589,7 +1606,7 @@
 </t>
         </is>
       </c>
-      <c r="N6" s="5" t="inlineStr"/>
+      <c r="N6" s="9" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="B7" s="2" t="n"/>

</xml_diff>